<commit_message>
New stations and updates to sheets
</commit_message>
<xml_diff>
--- a/LOCATION SHEETS/1677sLOCATIONS.xlsx
+++ b/LOCATION SHEETS/1677sLOCATIONS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Documents/WR4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD55660-272D-4348-B15F-B4649F4666AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48EFD5D-A266-0C40-A893-2F745054A453}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="460" windowWidth="28100" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2861" uniqueCount="1051">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2865" uniqueCount="1052">
   <si>
     <t>LOCATIONS FOR MIXTURE OF DECADES</t>
   </si>
@@ -4091,6 +4091,9 @@
   </si>
   <si>
     <t>RR500</t>
+  </si>
+  <si>
+    <t>RR501</t>
   </si>
 </sst>
 </file>
@@ -4334,7 +4337,39 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4842,9 +4877,9 @@
   </sheetPr>
   <dimension ref="A1:K1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I224" sqref="I224"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I226" sqref="I226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -6840,6 +6875,9 @@
       <c r="G76" s="30">
         <v>1780</v>
       </c>
+      <c r="H76" t="s">
+        <v>1051</v>
+      </c>
       <c r="J76" s="28" t="s">
         <v>161</v>
       </c>
@@ -6867,6 +6905,9 @@
       <c r="G77" s="30">
         <v>1790</v>
       </c>
+      <c r="H77" t="s">
+        <v>1051</v>
+      </c>
       <c r="J77" s="28" t="s">
         <v>161</v>
       </c>
@@ -7086,6 +7127,9 @@
       <c r="G84" s="30">
         <v>1730</v>
       </c>
+      <c r="H84" s="42" t="s">
+        <v>1018</v>
+      </c>
       <c r="J84" s="28" t="s">
         <v>175</v>
       </c>
@@ -7113,6 +7157,9 @@
       <c r="G85" s="30">
         <v>1730</v>
       </c>
+      <c r="H85" s="42" t="s">
+        <v>1018</v>
+      </c>
       <c r="J85" s="28" t="s">
         <v>175</v>
       </c>
@@ -9110,6 +9157,7 @@
       <c r="H161" t="s">
         <v>1048</v>
       </c>
+      <c r="I161" s="23"/>
       <c r="J161" s="28" t="s">
         <v>315</v>
       </c>
@@ -9125,8 +9173,8 @@
         <v>160</v>
       </c>
       <c r="C162" s="25"/>
-      <c r="D162" s="23" t="s">
-        <v>307</v>
+      <c r="D162" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="E162" s="26"/>
       <c r="F162" s="28" t="s">
@@ -9135,8 +9183,8 @@
       <c r="G162" s="30">
         <v>1810</v>
       </c>
-      <c r="H162" t="s">
-        <v>1048</v>
+      <c r="I162" s="4" t="s">
+        <v>307</v>
       </c>
       <c r="J162" s="28" t="s">
         <v>308</v>
@@ -22382,123 +22430,143 @@
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
   <conditionalFormatting sqref="I98 I206:I207 D1:D1006">
-    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="Disagreement">
+    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="Disagreement">
       <formula>NOT(ISERROR(SEARCH(("Disagreement"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:G1006">
-    <cfRule type="containsBlanks" dxfId="22" priority="22">
+    <cfRule type="containsBlanks" dxfId="26" priority="26">
       <formula>LEN(TRIM(G7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I98 I206:I207 D7:D1006">
-    <cfRule type="containsBlanks" dxfId="21" priority="23">
+    <cfRule type="containsBlanks" dxfId="25" priority="27">
       <formula>LEN(TRIM(D7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C1006">
-    <cfRule type="containsBlanks" dxfId="20" priority="24">
+    <cfRule type="containsBlanks" dxfId="24" priority="28">
       <formula>LEN(TRIM(C7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I379">
-    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="Disagreement">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Disagreement">
       <formula>NOT(ISERROR(SEARCH(("Disagreement"),(I379))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I379">
-    <cfRule type="containsBlanks" dxfId="18" priority="20">
+    <cfRule type="containsBlanks" dxfId="22" priority="24">
       <formula>LEN(TRIM(I379))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I156">
-    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="Disagreement">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Disagreement">
       <formula>NOT(ISERROR(SEARCH(("Disagreement"),(I156))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I156">
-    <cfRule type="containsBlanks" dxfId="16" priority="18">
+    <cfRule type="containsBlanks" dxfId="20" priority="22">
       <formula>LEN(TRIM(I156))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I453">
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Disagreement">
+    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="Disagreement">
       <formula>NOT(ISERROR(SEARCH(("Disagreement"),(I453))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I453">
-    <cfRule type="containsBlanks" dxfId="14" priority="16">
+    <cfRule type="containsBlanks" dxfId="18" priority="20">
       <formula>LEN(TRIM(I453))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I293">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Disagreement">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="Disagreement">
       <formula>NOT(ISERROR(SEARCH(("Disagreement"),(I293))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I293">
-    <cfRule type="containsBlanks" dxfId="12" priority="14">
+    <cfRule type="containsBlanks" dxfId="16" priority="18">
       <formula>LEN(TRIM(I293))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I292">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="Disagreement">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Disagreement">
       <formula>NOT(ISERROR(SEARCH(("Disagreement"),(I292))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I292">
-    <cfRule type="containsBlanks" dxfId="10" priority="12">
+    <cfRule type="containsBlanks" dxfId="14" priority="16">
       <formula>LEN(TRIM(I292))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I294">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Disagreement">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Disagreement">
       <formula>NOT(ISERROR(SEARCH(("Disagreement"),(I294))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I294">
-    <cfRule type="containsBlanks" dxfId="8" priority="10">
+    <cfRule type="containsBlanks" dxfId="12" priority="14">
       <formula>LEN(TRIM(I294))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I295">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Disagreement">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="Disagreement">
       <formula>NOT(ISERROR(SEARCH(("Disagreement"),(I295))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I295">
-    <cfRule type="containsBlanks" dxfId="6" priority="8">
+    <cfRule type="containsBlanks" dxfId="10" priority="12">
       <formula>LEN(TRIM(I295))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I350">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Disagreement">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Disagreement">
       <formula>NOT(ISERROR(SEARCH(("Disagreement"),(I350))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I350">
-    <cfRule type="containsBlanks" dxfId="4" priority="6">
+    <cfRule type="containsBlanks" dxfId="8" priority="10">
       <formula>LEN(TRIM(I350))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I349">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Disagreement">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Disagreement">
       <formula>NOT(ISERROR(SEARCH(("Disagreement"),(I349))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I349">
-    <cfRule type="containsBlanks" dxfId="2" priority="4">
+    <cfRule type="containsBlanks" dxfId="6" priority="8">
       <formula>LEN(TRIM(I349))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I475">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Disagreement">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Disagreement">
       <formula>NOT(ISERROR(SEARCH(("Disagreement"),(I475))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I475">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
+      <formula>LEN(TRIM(I475))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I161">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Disagreement">
+      <formula>NOT(ISERROR(SEARCH(("Disagreement"),(I161))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I161">
+    <cfRule type="containsBlanks" dxfId="2" priority="4">
+      <formula>LEN(TRIM(I161))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I162">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Disagreement">
+      <formula>NOT(ISERROR(SEARCH(("Disagreement"),(I162))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I162">
     <cfRule type="containsBlanks" dxfId="0" priority="2">
-      <formula>LEN(TRIM(I475))=0</formula>
+      <formula>LEN(TRIM(I162))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
More completed stations added and small fixes
</commit_message>
<xml_diff>
--- a/LOCATION SHEETS/1677sLOCATIONS.xlsx
+++ b/LOCATION SHEETS/1677sLOCATIONS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Documents/WR4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2902E9-91C7-1D41-A64A-E1D7F697C290}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4DC48E-6214-7345-A248-AF17248633C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="28100" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2740" yWindow="460" windowWidth="28100" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1677sLOCATIONS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2868" uniqueCount="1053">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="1058">
   <si>
     <t>LOCATIONS FOR MIXTURE OF DECADES</t>
   </si>
@@ -3130,9 +3130,6 @@
     </r>
   </si>
   <si>
-    <t>PETERHEAD</t>
-  </si>
-  <si>
     <t>May 1808 to end 1809</t>
   </si>
   <si>
@@ -3919,9 +3916,6 @@
     <t>RR315</t>
   </si>
   <si>
-    <t>RR324</t>
-  </si>
-  <si>
     <t>DERBY (SWANWICK)</t>
   </si>
   <si>
@@ -4069,9 +4063,6 @@
     <t>RR460</t>
   </si>
   <si>
-    <t>Chelmsford (High St)</t>
-  </si>
-  <si>
     <t>RR494</t>
   </si>
   <si>
@@ -4093,10 +4084,34 @@
     <t>CAMDEN TOWN (Joyce)</t>
   </si>
   <si>
-    <t xml:space="preserve">MALTON UNKNOWN </t>
-  </si>
-  <si>
     <t>MALTON UNKNOWN</t>
+  </si>
+  <si>
+    <t>Chelmsford (BRITTON)</t>
+  </si>
+  <si>
+    <t>EDINBURGH UNKNOWN</t>
+  </si>
+  <si>
+    <t>RR502</t>
+  </si>
+  <si>
+    <t>RR503</t>
+  </si>
+  <si>
+    <t>RR504</t>
+  </si>
+  <si>
+    <t>RR505</t>
+  </si>
+  <si>
+    <t>RR506</t>
+  </si>
+  <si>
+    <t>MALTON</t>
+  </si>
+  <si>
+    <t>PETERHEAD (EARLY)</t>
   </si>
 </sst>
 </file>
@@ -4881,8 +4896,8 @@
   <dimension ref="A1:K1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A409" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I434" sqref="I434"/>
+      <pane ySplit="6" topLeftCell="A471" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I491" sqref="I491"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -5071,7 +5086,7 @@
         <v>1790</v>
       </c>
       <c r="H9" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="J9" s="28" t="s">
         <v>25</v>
@@ -5101,7 +5116,7 @@
         <v>1800</v>
       </c>
       <c r="H10" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="I10" s="28" t="s">
         <v>27</v>
@@ -5134,7 +5149,7 @@
         <v>1810</v>
       </c>
       <c r="H11" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="J11" s="28" t="s">
         <v>25</v>
@@ -5161,8 +5176,8 @@
       <c r="G12" s="30">
         <v>1770</v>
       </c>
-      <c r="H12" t="s">
-        <v>970</v>
+      <c r="H12" s="42" t="s">
+        <v>1010</v>
       </c>
       <c r="K12" s="28" t="s">
         <v>33</v>
@@ -5187,7 +5202,7 @@
         <v>1780</v>
       </c>
       <c r="H13" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I13" s="28" t="s">
         <v>34</v>
@@ -5217,7 +5232,7 @@
         <v>1780</v>
       </c>
       <c r="H14" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="J14" s="28" t="s">
         <v>38</v>
@@ -5437,7 +5452,7 @@
         <v>1790</v>
       </c>
       <c r="H22" s="42" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="I22" s="28" t="s">
         <v>51</v>
@@ -5492,7 +5507,7 @@
         <v>1790</v>
       </c>
       <c r="H24" s="42" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="I24" s="28" t="s">
         <v>56</v>
@@ -5525,7 +5540,7 @@
         <v>1800</v>
       </c>
       <c r="H25" s="42" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="J25" s="28" t="s">
         <v>52</v>
@@ -5555,7 +5570,7 @@
         <v>1720</v>
       </c>
       <c r="H26" s="42" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="J26" s="28" t="s">
         <v>60</v>
@@ -5585,7 +5600,7 @@
         <v>1720</v>
       </c>
       <c r="H27" s="42" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="I27" s="28" t="s">
         <v>62</v>
@@ -5618,7 +5633,7 @@
         <v>1730</v>
       </c>
       <c r="H28" s="42" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="I28" s="28" t="s">
         <v>62</v>
@@ -5651,7 +5666,7 @@
         <v>1730</v>
       </c>
       <c r="H29" s="42" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="J29" s="28" t="s">
         <v>60</v>
@@ -5681,7 +5696,7 @@
         <v>1770</v>
       </c>
       <c r="H30" s="42" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="I30" s="28" t="s">
         <v>62</v>
@@ -5714,7 +5729,7 @@
         <v>1760</v>
       </c>
       <c r="H31" s="42" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="J31" s="28" t="s">
         <v>68</v>
@@ -5798,7 +5813,7 @@
         <v>1780</v>
       </c>
       <c r="H34" s="42" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="J34" s="28" t="s">
         <v>73</v>
@@ -5828,7 +5843,7 @@
         <v>1790</v>
       </c>
       <c r="H35" s="42" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="I35" s="28" t="s">
         <v>75</v>
@@ -5940,7 +5955,7 @@
         <v>1800</v>
       </c>
       <c r="I39" s="42" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="J39" s="28" t="s">
         <v>84</v>
@@ -5970,7 +5985,7 @@
         <v>1810</v>
       </c>
       <c r="H40" s="42" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="K40" s="32" t="s">
         <v>88</v>
@@ -5995,7 +6010,7 @@
         <v>1810</v>
       </c>
       <c r="H41" s="42" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="I41" s="6" t="s">
         <v>87</v>
@@ -6025,7 +6040,7 @@
         <v>1800</v>
       </c>
       <c r="H42" s="42" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="J42" s="28" t="s">
         <v>90</v>
@@ -6341,10 +6356,10 @@
         <v>1720</v>
       </c>
       <c r="H55" s="42" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="I55" s="42" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="K55" s="28" t="s">
         <v>116</v>
@@ -6371,7 +6386,7 @@
         <v>1730</v>
       </c>
       <c r="I56" s="42" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="J56" s="28" t="s">
         <v>118</v>
@@ -6401,7 +6416,7 @@
         <v>1740</v>
       </c>
       <c r="I57" s="42" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="J57" s="28" t="s">
         <v>118</v>
@@ -6431,7 +6446,7 @@
         <v>1750</v>
       </c>
       <c r="I58" s="42" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="J58" s="28" t="s">
         <v>118</v>
@@ -6461,7 +6476,7 @@
         <v>1760</v>
       </c>
       <c r="I59" s="42" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="J59" s="28" t="s">
         <v>118</v>
@@ -6684,6 +6699,9 @@
       <c r="G68" s="30">
         <v>1780</v>
       </c>
+      <c r="H68" t="s">
+        <v>1053</v>
+      </c>
       <c r="K68" s="28" t="s">
         <v>142</v>
       </c>
@@ -6706,6 +6724,9 @@
       <c r="G69" s="30">
         <v>1790</v>
       </c>
+      <c r="H69" t="s">
+        <v>1053</v>
+      </c>
       <c r="K69" s="28" t="s">
         <v>143</v>
       </c>
@@ -6750,6 +6771,9 @@
       <c r="G71" s="30">
         <v>1780</v>
       </c>
+      <c r="H71" t="s">
+        <v>1053</v>
+      </c>
       <c r="K71" s="28" t="s">
         <v>147</v>
       </c>
@@ -6819,7 +6843,7 @@
         <v>1790</v>
       </c>
       <c r="H74" s="42" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="J74" s="28" t="s">
         <v>153</v>
@@ -6849,7 +6873,7 @@
         <v>1810</v>
       </c>
       <c r="H75" s="42" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="I75" s="28" t="s">
         <v>156</v>
@@ -6882,7 +6906,7 @@
         <v>1780</v>
       </c>
       <c r="H76" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="J76" s="28" t="s">
         <v>160</v>
@@ -6912,7 +6936,7 @@
         <v>1790</v>
       </c>
       <c r="H77" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="J77" s="28" t="s">
         <v>160</v>
@@ -7041,7 +7065,7 @@
         <v>1820</v>
       </c>
       <c r="H81" s="42" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="I81" s="28" t="s">
         <v>170</v>
@@ -7074,7 +7098,7 @@
         <v>1720</v>
       </c>
       <c r="H82" s="42" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="J82" s="28" t="s">
         <v>174</v>
@@ -7104,7 +7128,7 @@
         <v>1720</v>
       </c>
       <c r="H83" s="42" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="J83" s="28" t="s">
         <v>174</v>
@@ -7134,7 +7158,7 @@
         <v>1730</v>
       </c>
       <c r="H84" s="42" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="J84" s="28" t="s">
         <v>174</v>
@@ -7164,7 +7188,7 @@
         <v>1730</v>
       </c>
       <c r="H85" s="42" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="J85" s="28" t="s">
         <v>174</v>
@@ -7447,7 +7471,7 @@
         <v>1770</v>
       </c>
       <c r="H96" s="42" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="J96" s="28" t="s">
         <v>205</v>
@@ -7553,6 +7577,9 @@
       <c r="G100" s="30">
         <v>1740</v>
       </c>
+      <c r="H100" t="s">
+        <v>1054</v>
+      </c>
       <c r="K100" s="28" t="s">
         <v>213</v>
       </c>
@@ -7575,11 +7602,9 @@
       <c r="G101" s="30">
         <v>1740</v>
       </c>
-      <c r="H101" s="42" t="s">
-        <v>296</v>
-      </c>
+      <c r="H101" s="42"/>
       <c r="I101" s="42" t="s">
-        <v>1051</v>
+        <v>1056</v>
       </c>
       <c r="K101" s="28" t="s">
         <v>214</v>
@@ -7663,6 +7688,9 @@
       <c r="G104" s="30">
         <v>1790</v>
       </c>
+      <c r="H104" t="s">
+        <v>1055</v>
+      </c>
       <c r="K104" s="28" t="s">
         <v>222</v>
       </c>
@@ -7685,6 +7713,9 @@
       <c r="G105" s="30">
         <v>1790</v>
       </c>
+      <c r="H105" t="s">
+        <v>1055</v>
+      </c>
       <c r="K105" s="28" t="s">
         <v>223</v>
       </c>
@@ -7734,7 +7765,7 @@
         <v>1780</v>
       </c>
       <c r="H107" s="42" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="J107" s="28" t="s">
         <v>228</v>
@@ -7764,7 +7795,7 @@
         <v>1790</v>
       </c>
       <c r="H108" s="42" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="J108" s="28" t="s">
         <v>228</v>
@@ -7793,11 +7824,8 @@
       <c r="G109" s="30">
         <v>1740</v>
       </c>
-      <c r="H109">
-        <v>1291</v>
-      </c>
       <c r="I109" t="s">
-        <v>1043</v>
+        <v>1049</v>
       </c>
       <c r="J109" s="28" t="s">
         <v>232</v>
@@ -7827,7 +7855,7 @@
         <v>1690</v>
       </c>
       <c r="H110" s="42" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="J110" s="28" t="s">
         <v>235</v>
@@ -7857,7 +7885,7 @@
         <v>1690</v>
       </c>
       <c r="H111" s="42" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="I111" s="28" t="s">
         <v>237</v>
@@ -7890,7 +7918,7 @@
         <v>1700</v>
       </c>
       <c r="H112" s="42" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="J112" s="28" t="s">
         <v>235</v>
@@ -7920,7 +7948,7 @@
         <v>1700</v>
       </c>
       <c r="H113" s="42" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="I113" s="28" t="s">
         <v>237</v>
@@ -7953,7 +7981,7 @@
         <v>1710</v>
       </c>
       <c r="H114" s="42" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="I114" s="28" t="s">
         <v>242</v>
@@ -7986,7 +8014,7 @@
         <v>1710</v>
       </c>
       <c r="H115" s="42" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="I115" s="28" t="s">
         <v>244</v>
@@ -8029,7 +8057,7 @@
       </c>
       <c r="C117" s="25"/>
       <c r="D117" s="4" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="E117" s="26"/>
       <c r="F117" s="28" t="s">
@@ -8108,10 +8136,10 @@
         <v>1720</v>
       </c>
       <c r="H120" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="I120" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="K120" s="28" t="s">
         <v>251</v>
@@ -8137,8 +8165,11 @@
       <c r="G121" s="30">
         <v>1720</v>
       </c>
+      <c r="H121" t="s">
+        <v>1033</v>
+      </c>
       <c r="I121" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="K121" s="28" t="s">
         <v>253</v>
@@ -8162,8 +8193,11 @@
       <c r="G122" s="30">
         <v>1730</v>
       </c>
+      <c r="H122" t="s">
+        <v>1033</v>
+      </c>
       <c r="I122" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="K122" s="28" t="s">
         <v>254</v>
@@ -8189,8 +8223,11 @@
       <c r="G123" s="30">
         <v>1740</v>
       </c>
+      <c r="H123" t="s">
+        <v>1033</v>
+      </c>
       <c r="I123" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="K123" s="28" t="s">
         <v>255</v>
@@ -8216,8 +8253,11 @@
       <c r="G124" s="30">
         <v>1750</v>
       </c>
+      <c r="H124" t="s">
+        <v>1033</v>
+      </c>
       <c r="I124" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="K124" s="28" t="s">
         <v>256</v>
@@ -8341,8 +8381,11 @@
       <c r="G129" s="30">
         <v>1730</v>
       </c>
+      <c r="H129" t="s">
+        <v>1033</v>
+      </c>
       <c r="I129" s="6" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="K129" s="28" t="s">
         <v>255</v>
@@ -8369,7 +8412,7 @@
         <v>1760</v>
       </c>
       <c r="H130" s="42" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="I130" s="28" t="s">
         <v>267</v>
@@ -8402,7 +8445,7 @@
         <v>1760</v>
       </c>
       <c r="H131" s="42" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="I131" s="28" t="s">
         <v>270</v>
@@ -8432,7 +8475,7 @@
         <v>1770</v>
       </c>
       <c r="H132" s="42" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="I132" s="28" t="s">
         <v>270</v>
@@ -8578,7 +8621,7 @@
         <v>1770</v>
       </c>
       <c r="H138" s="42" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="K138" s="28" t="s">
         <v>284</v>
@@ -8603,7 +8646,7 @@
         <v>1770</v>
       </c>
       <c r="H139" s="42" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="K139" s="28" t="s">
         <v>286</v>
@@ -8628,7 +8671,7 @@
         <v>1780</v>
       </c>
       <c r="H140" s="42" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="K140" s="28" t="s">
         <v>287</v>
@@ -8653,7 +8696,7 @@
         <v>1790</v>
       </c>
       <c r="H141" s="42" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="K141" s="28" t="s">
         <v>287</v>
@@ -8752,7 +8795,7 @@
         <v>1730</v>
       </c>
       <c r="H145" s="42" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="I145" s="28" t="s">
         <v>297</v>
@@ -8779,7 +8822,7 @@
         <v>1730</v>
       </c>
       <c r="H146" s="42" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="I146" s="28" t="s">
         <v>297</v>
@@ -8806,7 +8849,7 @@
         <v>1740</v>
       </c>
       <c r="H147" s="42" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="148" spans="1:11" ht="13">
@@ -8830,7 +8873,7 @@
         <v>1750</v>
       </c>
       <c r="H148" s="42" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="I148" s="28" t="s">
         <v>297</v>
@@ -8857,7 +8900,7 @@
         <v>1760</v>
       </c>
       <c r="H149" s="42" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="150" spans="1:11" ht="13">
@@ -8881,7 +8924,7 @@
         <v>1770</v>
       </c>
       <c r="H150" s="42" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="151" spans="1:11" ht="13">
@@ -8905,7 +8948,7 @@
         <v>1770</v>
       </c>
       <c r="H151" s="42" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="152" spans="1:11" ht="13">
@@ -8929,7 +8972,7 @@
         <v>1780</v>
       </c>
       <c r="H152" s="42" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="I152" s="28" t="s">
         <v>297</v>
@@ -8956,7 +8999,7 @@
         <v>1790</v>
       </c>
       <c r="H153" s="42" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="154" spans="1:11" ht="13">
@@ -8980,7 +9023,7 @@
         <v>1800</v>
       </c>
       <c r="H154" s="42" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="155" spans="1:11" ht="13">
@@ -9017,7 +9060,7 @@
       </c>
       <c r="C156" s="25"/>
       <c r="D156" s="4" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="E156" s="26"/>
       <c r="F156" s="28" t="s">
@@ -9027,7 +9070,7 @@
         <v>1800</v>
       </c>
       <c r="I156" s="4" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="J156" s="28" t="s">
         <v>303</v>
@@ -9107,7 +9150,7 @@
         <v>1790</v>
       </c>
       <c r="H159" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="J159" s="28" t="s">
         <v>313</v>
@@ -9137,7 +9180,7 @@
         <v>1800</v>
       </c>
       <c r="H160" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="J160" s="28" t="s">
         <v>313</v>
@@ -9167,7 +9210,7 @@
         <v>1800</v>
       </c>
       <c r="H161" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="I161" s="23"/>
       <c r="J161" s="28" t="s">
@@ -9465,7 +9508,7 @@
         <v>1810</v>
       </c>
       <c r="I171" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="J171" s="28" t="s">
         <v>333</v>
@@ -9520,7 +9563,7 @@
         <v>1830</v>
       </c>
       <c r="H173" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="I173" s="28" t="s">
         <v>339</v>
@@ -9553,7 +9596,7 @@
         <v>1840</v>
       </c>
       <c r="H174" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="I174" s="28" t="s">
         <v>339</v>
@@ -9584,7 +9627,7 @@
         <v>1770</v>
       </c>
       <c r="H175" s="42" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="K175" s="28" t="s">
         <v>344</v>
@@ -9611,7 +9654,7 @@
         <v>1770</v>
       </c>
       <c r="H176" s="42" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="J176" s="28" t="s">
         <v>346</v>
@@ -9641,7 +9684,7 @@
         <v>1770</v>
       </c>
       <c r="H177" s="42" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="K177" s="28" t="s">
         <v>347</v>
@@ -9668,7 +9711,7 @@
         <v>1780</v>
       </c>
       <c r="H178" s="42" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="K178" s="28" t="s">
         <v>348</v>
@@ -9693,7 +9736,7 @@
         <v>1780</v>
       </c>
       <c r="H179" s="42" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="K179" s="28" t="s">
         <v>349</v>
@@ -9720,7 +9763,7 @@
         <v>1780</v>
       </c>
       <c r="H180" s="42" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="K180" s="28" t="s">
         <v>348</v>
@@ -9747,7 +9790,7 @@
         <v>1790</v>
       </c>
       <c r="H181" s="42" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="J181" s="28" t="s">
         <v>346</v>
@@ -9797,7 +9840,7 @@
         <v>1780</v>
       </c>
       <c r="H183" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="I183" s="28" t="s">
         <v>354</v>
@@ -9872,10 +9915,10 @@
         <v>1800</v>
       </c>
       <c r="H186" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="I186" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="K186" s="28" t="s">
         <v>357</v>
@@ -9900,7 +9943,7 @@
         <v>1810</v>
       </c>
       <c r="I187" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="K187" s="28" t="s">
         <v>358</v>
@@ -9925,7 +9968,7 @@
         <v>1790</v>
       </c>
       <c r="H188" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="I188" s="28" t="s">
         <v>359</v>
@@ -10155,7 +10198,7 @@
         <v>1830</v>
       </c>
       <c r="H197" s="42" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="J197" s="28" t="s">
         <v>370</v>
@@ -10185,7 +10228,7 @@
         <v>1840</v>
       </c>
       <c r="H198" s="42" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="J198" s="28" t="s">
         <v>370</v>
@@ -10215,7 +10258,7 @@
         <v>1830</v>
       </c>
       <c r="H199" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="K199" s="28" t="s">
         <v>375</v>
@@ -10242,7 +10285,7 @@
         <v>1840</v>
       </c>
       <c r="H200" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="I200" s="28" t="s">
         <v>376</v>
@@ -10294,7 +10337,7 @@
         <v>1670</v>
       </c>
       <c r="H202" s="6" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="J202" s="28" t="s">
         <v>382</v>
@@ -10324,7 +10367,7 @@
         <v>1680</v>
       </c>
       <c r="H203" s="6" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="J203" s="28" t="s">
         <v>382</v>
@@ -10354,7 +10397,7 @@
         <v>1680</v>
       </c>
       <c r="H204" s="6" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="I204" s="28" t="s">
         <v>386</v>
@@ -10387,7 +10430,7 @@
         <v>1690</v>
       </c>
       <c r="H205" s="6" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="J205" s="28" t="s">
         <v>382</v>
@@ -10417,7 +10460,7 @@
         <v>1690</v>
       </c>
       <c r="H206" s="6" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="I206" s="28" t="s">
         <v>381</v>
@@ -10450,7 +10493,7 @@
         <v>1700</v>
       </c>
       <c r="H207" s="6" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="I207" s="28" t="s">
         <v>389</v>
@@ -10481,7 +10524,7 @@
         <v>1780</v>
       </c>
       <c r="H208" s="6" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="K208" s="28" t="s">
         <v>392</v>
@@ -10655,10 +10698,10 @@
         <v>1780</v>
       </c>
       <c r="H215" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="I215" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="K215" s="28" t="s">
         <v>402</v>
@@ -10683,7 +10726,7 @@
         <v>1780</v>
       </c>
       <c r="I216" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="K216" s="28" t="s">
         <v>403</v>
@@ -10708,7 +10751,7 @@
         <v>1790</v>
       </c>
       <c r="I217" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="K217" s="28" t="s">
         <v>404</v>
@@ -10733,7 +10776,7 @@
         <v>1790</v>
       </c>
       <c r="I218" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="K218" s="28" t="s">
         <v>405</v>
@@ -10760,7 +10803,7 @@
         <v>1790</v>
       </c>
       <c r="I219" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="K219" s="28" t="s">
         <v>407</v>
@@ -10785,7 +10828,7 @@
         <v>1790</v>
       </c>
       <c r="I220" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="K220" s="28" t="s">
         <v>394</v>
@@ -10812,7 +10855,7 @@
         <v>1820</v>
       </c>
       <c r="H221" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="K221" s="28" t="s">
         <v>410</v>
@@ -10884,7 +10927,7 @@
         <v>1820</v>
       </c>
       <c r="H224" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="J224" s="28" t="s">
         <v>414</v>
@@ -10911,7 +10954,7 @@
         <v>1830</v>
       </c>
       <c r="H225" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="J225" s="28" t="s">
         <v>414</v>
@@ -10936,7 +10979,7 @@
         <v>1840</v>
       </c>
       <c r="H226" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="I226" s="28" t="s">
         <v>417</v>
@@ -10963,7 +11006,7 @@
         <v>1830</v>
       </c>
       <c r="H227" s="6" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="J227" s="28" t="s">
         <v>420</v>
@@ -10993,7 +11036,7 @@
         <v>1840</v>
       </c>
       <c r="H228" s="6" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="J228" s="28" t="s">
         <v>420</v>
@@ -11033,10 +11076,10 @@
         <v>1770</v>
       </c>
       <c r="H230" s="42" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="I230" s="42" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="K230" s="28" t="s">
         <v>425</v>
@@ -11061,7 +11104,7 @@
         <v>1780</v>
       </c>
       <c r="I231" s="42" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="K231" s="28" t="s">
         <v>426</v>
@@ -11088,7 +11131,7 @@
         <v>1820</v>
       </c>
       <c r="H232" s="42" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="I232" s="28" t="s">
         <v>428</v>
@@ -11118,7 +11161,7 @@
         <v>1830</v>
       </c>
       <c r="H233" s="42" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="I233" s="28" t="s">
         <v>428</v>
@@ -11148,7 +11191,7 @@
         <v>1840</v>
       </c>
       <c r="H234" s="42" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="I234" s="28" t="s">
         <v>428</v>
@@ -11260,7 +11303,7 @@
         <v>1830</v>
       </c>
       <c r="H238" s="42" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="I238" s="28" t="s">
         <v>434</v>
@@ -11293,7 +11336,7 @@
         <v>1840</v>
       </c>
       <c r="H239" s="42" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="I239" s="28" t="s">
         <v>434</v>
@@ -11326,7 +11369,7 @@
         <v>1830</v>
       </c>
       <c r="H240" s="42" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="J240" s="28" t="s">
         <v>438</v>
@@ -11766,7 +11809,7 @@
         <v>1870</v>
       </c>
       <c r="H257" s="42" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="J257" s="28" t="s">
         <v>482</v>
@@ -12067,7 +12110,7 @@
         <v>1750</v>
       </c>
       <c r="H268" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="I268" s="28" t="s">
         <v>508</v>
@@ -12209,10 +12252,10 @@
         <v>1800</v>
       </c>
       <c r="H273" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="I273" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="K273" s="28" t="s">
         <v>516</v>
@@ -12237,7 +12280,7 @@
         <v>1810</v>
       </c>
       <c r="I274" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="K274" s="28" t="s">
         <v>517</v>
@@ -12262,7 +12305,7 @@
         <v>1820</v>
       </c>
       <c r="I275" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="K275" s="28" t="s">
         <v>518</v>
@@ -12336,10 +12379,10 @@
         <v>1780</v>
       </c>
       <c r="H278" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="I278" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="J278" s="28" t="s">
         <v>525</v>
@@ -12367,7 +12410,7 @@
         <v>1780</v>
       </c>
       <c r="I279" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="K279" s="28" t="s">
         <v>527</v>
@@ -12392,7 +12435,7 @@
         <v>1790</v>
       </c>
       <c r="I280" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="K280" s="28" t="s">
         <v>528</v>
@@ -12419,7 +12462,7 @@
         <v>1790</v>
       </c>
       <c r="I281" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="K281" s="28" t="s">
         <v>530</v>
@@ -12444,7 +12487,7 @@
         <v>1790</v>
       </c>
       <c r="I282" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="K282" s="28" t="s">
         <v>531</v>
@@ -12497,7 +12540,7 @@
         <v>1790</v>
       </c>
       <c r="I284" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="K284" s="28" t="s">
         <v>535</v>
@@ -12522,7 +12565,7 @@
         <v>1800</v>
       </c>
       <c r="I285" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="K285" s="28" t="s">
         <v>536</v>
@@ -12720,10 +12763,10 @@
         <v>1770</v>
       </c>
       <c r="H292" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="I292" s="4" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="K292" s="28" t="s">
         <v>550</v>
@@ -12750,10 +12793,10 @@
         <v>1770</v>
       </c>
       <c r="H293" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="I293" s="4" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="K293" s="28" t="s">
         <v>551</v>
@@ -12778,10 +12821,10 @@
         <v>1780</v>
       </c>
       <c r="H294" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="I294" s="4" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="K294" s="28" t="s">
         <v>552</v>
@@ -12806,10 +12849,10 @@
         <v>1790</v>
       </c>
       <c r="H295" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="I295" s="4" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="K295" s="28" t="s">
         <v>553</v>
@@ -12920,7 +12963,7 @@
         <v>1770</v>
       </c>
       <c r="H299" s="42" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="J299" s="28" t="s">
         <v>565</v>
@@ -12950,7 +12993,7 @@
         <v>1780</v>
       </c>
       <c r="H300" s="42" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="J300" s="28" t="s">
         <v>565</v>
@@ -13042,7 +13085,7 @@
         <v>1760</v>
       </c>
       <c r="H303" s="42" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="K303" s="28" t="s">
         <v>576</v>
@@ -13069,7 +13112,7 @@
         <v>1770</v>
       </c>
       <c r="H304" s="42" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="K304" s="28" t="s">
         <v>326</v>
@@ -13118,6 +13161,9 @@
       <c r="G306" s="30">
         <v>1770</v>
       </c>
+      <c r="H306" t="s">
+        <v>1052</v>
+      </c>
       <c r="I306" s="28" t="s">
         <v>579</v>
       </c>
@@ -13146,6 +13192,9 @@
       <c r="G307" s="30">
         <v>1770</v>
       </c>
+      <c r="H307" t="s">
+        <v>1052</v>
+      </c>
       <c r="I307" s="28" t="s">
         <v>582</v>
       </c>
@@ -13218,6 +13267,9 @@
       <c r="G310" s="30">
         <v>1780</v>
       </c>
+      <c r="H310" t="s">
+        <v>1051</v>
+      </c>
       <c r="I310" s="28" t="s">
         <v>587</v>
       </c>
@@ -13245,6 +13297,9 @@
       <c r="G311" s="30">
         <v>1790</v>
       </c>
+      <c r="H311" t="s">
+        <v>1051</v>
+      </c>
       <c r="I311" s="6" t="s">
         <v>587</v>
       </c>
@@ -13369,8 +13424,8 @@
         <v>92</v>
       </c>
       <c r="C316" s="25"/>
-      <c r="D316" s="23" t="s">
-        <v>584</v>
+      <c r="D316" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="E316" s="26"/>
       <c r="F316" s="28" t="s">
@@ -13379,6 +13434,9 @@
       <c r="G316" s="30">
         <v>1800</v>
       </c>
+      <c r="I316" t="s">
+        <v>1050</v>
+      </c>
       <c r="K316" s="28" t="s">
         <v>599</v>
       </c>
@@ -13539,7 +13597,7 @@
         <v>1810</v>
       </c>
       <c r="H323" s="42" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="I323" s="28" t="s">
         <v>610</v>
@@ -13665,7 +13723,7 @@
         <v>1810</v>
       </c>
       <c r="H328" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="J328" s="28" t="s">
         <v>621</v>
@@ -13975,7 +14033,7 @@
         <v>1770</v>
       </c>
       <c r="H339" s="42" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="I339" s="28" t="s">
         <v>647</v>
@@ -14008,7 +14066,7 @@
         <v>1780</v>
       </c>
       <c r="H340" s="42" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="I340" s="28" t="s">
         <v>647</v>
@@ -14039,7 +14097,7 @@
         <v>1830</v>
       </c>
       <c r="H341" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="K341" s="37" t="s">
         <v>652</v>
@@ -14066,7 +14124,7 @@
         <v>1840</v>
       </c>
       <c r="H342" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="K342" s="37" t="s">
         <v>377</v>
@@ -14181,7 +14239,7 @@
         <v>1790</v>
       </c>
       <c r="H347" s="42" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="K347" s="37" t="s">
         <v>661</v>
@@ -14206,7 +14264,7 @@
         <v>1800</v>
       </c>
       <c r="H348" s="42" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="K348" s="37" t="s">
         <v>662</v>
@@ -14231,7 +14289,7 @@
         <v>1710</v>
       </c>
       <c r="H349" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="I349" s="4" t="s">
         <v>663</v>
@@ -14284,7 +14342,7 @@
         <v>1840</v>
       </c>
       <c r="H351" s="42" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="K351" s="37" t="s">
         <v>666</v>
@@ -14309,7 +14367,7 @@
         <v>1850</v>
       </c>
       <c r="H352" s="42" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="K352" s="37" t="s">
         <v>667</v>
@@ -14359,7 +14417,7 @@
         <v>1840</v>
       </c>
       <c r="H354" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="K354" s="28" t="s">
         <v>671</v>
@@ -14384,7 +14442,7 @@
         <v>1850</v>
       </c>
       <c r="H355" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="I355" s="28" t="s">
         <v>670</v>
@@ -14488,7 +14546,7 @@
         <v>1800</v>
       </c>
       <c r="H359" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I359" s="28" t="s">
         <v>682</v>
@@ -14516,7 +14574,7 @@
         <v>1800</v>
       </c>
       <c r="H360" s="42" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="I360" s="28" t="s">
         <v>684</v>
@@ -14699,7 +14757,7 @@
         <v>1800</v>
       </c>
       <c r="H367" s="42" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="I367" s="28" t="s">
         <v>698</v>
@@ -14757,7 +14815,7 @@
         <v>1800</v>
       </c>
       <c r="H369" s="42" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="K369" s="37" t="s">
         <v>705</v>
@@ -14912,7 +14970,7 @@
         <v>1800</v>
       </c>
       <c r="H375" s="42" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="K375" s="28" t="s">
         <v>41</v>
@@ -14964,7 +15022,7 @@
         <v>1800</v>
       </c>
       <c r="H377" s="42" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="J377" s="28" t="s">
         <v>717</v>
@@ -15009,7 +15067,7 @@
       </c>
       <c r="C379" s="25"/>
       <c r="D379" s="4" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="E379" s="26"/>
       <c r="F379" s="28" t="s">
@@ -15019,7 +15077,7 @@
         <v>1800</v>
       </c>
       <c r="I379" s="4" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="K379" s="28" t="s">
         <v>721</v>
@@ -15137,7 +15195,7 @@
       </c>
       <c r="C384" s="25"/>
       <c r="D384" s="4" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="E384" s="26"/>
       <c r="F384" s="28" t="s">
@@ -15147,7 +15205,7 @@
         <v>1800</v>
       </c>
       <c r="I384" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="K384" s="28" t="s">
         <v>729</v>
@@ -15227,7 +15285,7 @@
         <v>1800</v>
       </c>
       <c r="H387" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="I387" t="s">
         <v>351</v>
@@ -15401,7 +15459,7 @@
         <v>1800</v>
       </c>
       <c r="H394" s="42" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="K394" s="37" t="s">
         <v>746</v>
@@ -15426,7 +15484,7 @@
         <v>1800</v>
       </c>
       <c r="H395" s="42" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="K395" s="37" t="s">
         <v>748</v>
@@ -15545,7 +15603,7 @@
         <v>1800</v>
       </c>
       <c r="H400" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="I400" s="6" t="s">
         <v>532</v>
@@ -15646,7 +15704,7 @@
         <v>1800</v>
       </c>
       <c r="H404" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="J404" s="28" t="s">
         <v>763</v>
@@ -15674,7 +15732,7 @@
         <v>1800</v>
       </c>
       <c r="H405" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="K405" s="28" t="s">
         <v>766</v>
@@ -15873,10 +15931,10 @@
         <v>1800</v>
       </c>
       <c r="H413" s="42" t="s">
+        <v>979</v>
+      </c>
+      <c r="I413" s="6" t="s">
         <v>980</v>
-      </c>
-      <c r="I413" s="6" t="s">
-        <v>981</v>
       </c>
       <c r="J413" s="28" t="s">
         <v>611</v>
@@ -15893,8 +15951,8 @@
         <v>56</v>
       </c>
       <c r="C414" s="25"/>
-      <c r="D414" s="23" t="s">
-        <v>779</v>
+      <c r="D414" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="E414" s="26"/>
       <c r="F414" s="28" t="s">
@@ -15903,8 +15961,11 @@
       <c r="G414" s="30">
         <v>1800</v>
       </c>
+      <c r="I414" t="s">
+        <v>1057</v>
+      </c>
       <c r="K414" s="28" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="415" spans="1:11" ht="13">
@@ -15916,7 +15977,7 @@
       </c>
       <c r="C415" s="25"/>
       <c r="D415" s="23" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E415" s="26"/>
       <c r="F415" s="28" t="s">
@@ -15926,7 +15987,7 @@
         <v>1800</v>
       </c>
       <c r="K415" s="28" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="416" spans="1:11" ht="13">
@@ -15950,10 +16011,10 @@
         <v>1800</v>
       </c>
       <c r="I416" s="28" t="s">
+        <v>782</v>
+      </c>
+      <c r="K416" s="28" t="s">
         <v>783</v>
-      </c>
-      <c r="K416" s="28" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="417" spans="1:11" ht="13">
@@ -15981,10 +16042,10 @@
         <v>656</v>
       </c>
       <c r="J417" s="36" t="s">
+        <v>784</v>
+      </c>
+      <c r="K417" s="37" t="s">
         <v>785</v>
-      </c>
-      <c r="K417" s="37" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="418" spans="1:11" ht="13">
@@ -15996,7 +16057,7 @@
       </c>
       <c r="C418" s="25"/>
       <c r="D418" s="23" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E418" s="26"/>
       <c r="F418" s="28" t="s">
@@ -16006,7 +16067,7 @@
         <v>1800</v>
       </c>
       <c r="K418" s="28" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="419" spans="1:11" ht="13">
@@ -16018,7 +16079,7 @@
       </c>
       <c r="C419" s="25"/>
       <c r="D419" s="23" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E419" s="26"/>
       <c r="F419" s="28" t="s">
@@ -16031,7 +16092,7 @@
         <v>6121</v>
       </c>
       <c r="K419" s="28" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="420" spans="1:11" ht="13">
@@ -16095,7 +16156,7 @@
         <v>1800</v>
       </c>
       <c r="K422" s="37" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="423" spans="1:11" ht="13">
@@ -16117,13 +16178,13 @@
         <v>1810</v>
       </c>
       <c r="I423" s="28" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="J423" s="28" t="s">
         <v>775</v>
       </c>
       <c r="K423" s="28" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="424" spans="1:11" ht="13">
@@ -16145,16 +16206,16 @@
         <v>1800</v>
       </c>
       <c r="H424" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="I424" s="6" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="J424" s="28" t="s">
+        <v>793</v>
+      </c>
+      <c r="K424" s="28" t="s">
         <v>794</v>
-      </c>
-      <c r="K424" s="28" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="425" spans="1:11" ht="13">
@@ -16176,16 +16237,16 @@
         <v>1810</v>
       </c>
       <c r="H425" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="I425" s="6" t="s">
+        <v>795</v>
+      </c>
+      <c r="J425" s="28" t="s">
+        <v>793</v>
+      </c>
+      <c r="K425" s="28" t="s">
         <v>796</v>
-      </c>
-      <c r="J425" s="28" t="s">
-        <v>794</v>
-      </c>
-      <c r="K425" s="28" t="s">
-        <v>797</v>
       </c>
     </row>
     <row r="426" spans="1:11" ht="13">
@@ -16207,13 +16268,13 @@
         <v>1810</v>
       </c>
       <c r="H426" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="I426" s="28" t="s">
+        <v>797</v>
+      </c>
+      <c r="K426" s="28" t="s">
         <v>798</v>
-      </c>
-      <c r="K426" s="28" t="s">
-        <v>799</v>
       </c>
     </row>
     <row r="427" spans="1:11" ht="13">
@@ -16225,7 +16286,7 @@
       </c>
       <c r="C427" s="25"/>
       <c r="D427" s="23" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E427" s="26"/>
       <c r="F427" s="28" t="s">
@@ -16235,7 +16296,7 @@
         <v>1820</v>
       </c>
       <c r="K427" s="28" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="428" spans="1:11" ht="13">
@@ -16257,10 +16318,10 @@
         <v>1810</v>
       </c>
       <c r="I428" s="28" t="s">
+        <v>800</v>
+      </c>
+      <c r="K428" s="28" t="s">
         <v>801</v>
-      </c>
-      <c r="K428" s="28" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="429" spans="1:11" ht="13">
@@ -16274,7 +16335,7 @@
         <v>368</v>
       </c>
       <c r="D429" s="23" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E429" s="26"/>
       <c r="F429" s="28" t="s">
@@ -16284,13 +16345,13 @@
         <v>1810</v>
       </c>
       <c r="H429" s="42" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="J429" s="28" t="s">
         <v>370</v>
       </c>
       <c r="K429" s="28" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="430" spans="1:11" ht="13">
@@ -16302,7 +16363,7 @@
       </c>
       <c r="C430" s="25"/>
       <c r="D430" s="23" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E430" s="26"/>
       <c r="F430" s="28" t="s">
@@ -16315,7 +16376,7 @@
         <v>2902</v>
       </c>
       <c r="K430" s="28" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="431" spans="1:11" ht="13">
@@ -16337,10 +16398,10 @@
         <v>1810</v>
       </c>
       <c r="H431" s="42" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="K431" s="28" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="432" spans="1:11" ht="13">
@@ -16352,7 +16413,7 @@
       </c>
       <c r="C432" s="25"/>
       <c r="D432" s="23" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E432" s="26"/>
       <c r="F432" s="28" t="s">
@@ -16362,10 +16423,10 @@
         <v>1810</v>
       </c>
       <c r="H432" s="42" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="K432" s="28" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="433" spans="1:11" ht="13">
@@ -16377,7 +16438,7 @@
       </c>
       <c r="C433" s="25"/>
       <c r="D433" s="23" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E433" s="26"/>
       <c r="F433" s="28" t="s">
@@ -16387,10 +16448,10 @@
         <v>1810</v>
       </c>
       <c r="J433" s="28" t="s">
+        <v>810</v>
+      </c>
+      <c r="K433" s="28" t="s">
         <v>811</v>
-      </c>
-      <c r="K433" s="28" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="434" spans="1:11" ht="13">
@@ -16412,10 +16473,10 @@
         <v>1800</v>
       </c>
       <c r="I434" s="6" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
       <c r="K434" s="37" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="435" spans="1:11" ht="13">
@@ -16427,7 +16488,7 @@
       </c>
       <c r="C435" s="25"/>
       <c r="D435" s="23" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E435" s="26"/>
       <c r="F435" s="28" t="s">
@@ -16437,7 +16498,7 @@
         <v>1810</v>
       </c>
       <c r="K435" s="28" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="436" spans="1:11" ht="13">
@@ -16459,7 +16520,7 @@
         <v>1810</v>
       </c>
       <c r="K436" s="28" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="437" spans="1:11" ht="13">
@@ -16471,7 +16532,7 @@
       </c>
       <c r="C437" s="25"/>
       <c r="D437" s="23" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E437" s="26"/>
       <c r="F437" s="28" t="s">
@@ -16481,7 +16542,7 @@
         <v>1810</v>
       </c>
       <c r="K437" s="28" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="438" spans="1:11" ht="13">
@@ -16493,7 +16554,7 @@
       </c>
       <c r="C438" s="25"/>
       <c r="D438" s="23" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E438" s="26"/>
       <c r="F438" s="28" t="s">
@@ -16503,7 +16564,7 @@
         <v>1810</v>
       </c>
       <c r="K438" s="28" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="439" spans="1:11" ht="13">
@@ -16515,7 +16576,7 @@
       </c>
       <c r="C439" s="25"/>
       <c r="D439" s="23" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E439" s="26"/>
       <c r="F439" s="28" t="s">
@@ -16525,10 +16586,10 @@
         <v>1810</v>
       </c>
       <c r="H439" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="K439" s="28" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="440" spans="1:11" ht="13">
@@ -16550,7 +16611,7 @@
         <v>1810</v>
       </c>
       <c r="K440" s="28" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="441" spans="1:11" ht="13">
@@ -16572,10 +16633,10 @@
         <v>1810</v>
       </c>
       <c r="I441" s="28" t="s">
+        <v>823</v>
+      </c>
+      <c r="K441" s="37" t="s">
         <v>824</v>
-      </c>
-      <c r="K441" s="37" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="442" spans="1:11" ht="13">
@@ -16587,7 +16648,7 @@
       </c>
       <c r="C442" s="25"/>
       <c r="D442" s="23" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="E442" s="26"/>
       <c r="F442" s="28" t="s">
@@ -16597,7 +16658,7 @@
         <v>1810</v>
       </c>
       <c r="K442" s="28" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="443" spans="1:11" ht="13">
@@ -16621,10 +16682,10 @@
         <v>1810</v>
       </c>
       <c r="I443" s="28" t="s">
+        <v>827</v>
+      </c>
+      <c r="K443" s="28" t="s">
         <v>828</v>
-      </c>
-      <c r="K443" s="28" t="s">
-        <v>829</v>
       </c>
     </row>
     <row r="444" spans="1:11" ht="13">
@@ -16635,7 +16696,7 @@
         <v>88</v>
       </c>
       <c r="C444" s="29" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D444" s="23" t="s">
         <v>20</v>
@@ -16648,7 +16709,7 @@
         <v>1810</v>
       </c>
       <c r="H444" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="I444" s="28" t="s">
         <v>27</v>
@@ -16657,7 +16718,7 @@
         <v>25</v>
       </c>
       <c r="K444" s="28" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="445" spans="1:11" ht="13">
@@ -16681,16 +16742,16 @@
         <v>1810</v>
       </c>
       <c r="H445" s="42" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="I445" s="28" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="J445" s="28" t="s">
         <v>153</v>
       </c>
       <c r="K445" s="28" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="446" spans="1:11" ht="13">
@@ -16702,10 +16763,10 @@
       </c>
       <c r="C446" s="25"/>
       <c r="D446" s="23" t="s">
+        <v>833</v>
+      </c>
+      <c r="E446" s="23" t="s">
         <v>834</v>
-      </c>
-      <c r="E446" s="23" t="s">
-        <v>835</v>
       </c>
       <c r="F446" s="28" t="s">
         <v>21</v>
@@ -16717,7 +16778,7 @@
         <v>17</v>
       </c>
       <c r="K446" s="28" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="447" spans="1:11" ht="13">
@@ -16729,7 +16790,7 @@
       </c>
       <c r="C447" s="25"/>
       <c r="D447" s="23" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="E447" s="26"/>
       <c r="F447" s="28" t="s">
@@ -16742,7 +16803,7 @@
         <v>17</v>
       </c>
       <c r="K447" s="28" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="448" spans="1:11" ht="13">
@@ -16764,10 +16825,10 @@
         <v>1810</v>
       </c>
       <c r="I448" s="28" t="s">
+        <v>838</v>
+      </c>
+      <c r="K448" s="28" t="s">
         <v>839</v>
-      </c>
-      <c r="K448" s="28" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="449" spans="1:11" ht="13">
@@ -16789,10 +16850,10 @@
         <v>1810</v>
       </c>
       <c r="H449" s="42" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="K449" s="28" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="450" spans="1:11" ht="13">
@@ -16804,10 +16865,10 @@
       </c>
       <c r="C450" s="25"/>
       <c r="D450" s="23" t="s">
+        <v>841</v>
+      </c>
+      <c r="E450" s="23" t="s">
         <v>842</v>
-      </c>
-      <c r="E450" s="23" t="s">
-        <v>843</v>
       </c>
       <c r="F450" s="28" t="s">
         <v>21</v>
@@ -16816,7 +16877,7 @@
         <v>1810</v>
       </c>
       <c r="K450" s="28" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="451" spans="1:11" ht="13">
@@ -16827,10 +16888,10 @@
         <v>95</v>
       </c>
       <c r="C451" s="29" t="s">
+        <v>844</v>
+      </c>
+      <c r="D451" s="23" t="s">
         <v>845</v>
-      </c>
-      <c r="D451" s="23" t="s">
-        <v>846</v>
       </c>
       <c r="E451" s="26"/>
       <c r="F451" s="28" t="s">
@@ -16840,7 +16901,7 @@
         <v>1810</v>
       </c>
       <c r="K451" s="28" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="452" spans="1:11" ht="13">
@@ -16852,7 +16913,7 @@
       </c>
       <c r="C452" s="25"/>
       <c r="D452" s="23" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="E452" s="26"/>
       <c r="F452" s="28" t="s">
@@ -16862,7 +16923,7 @@
         <v>1810</v>
       </c>
       <c r="K452" s="28" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="453" spans="1:11" ht="13">
@@ -16884,13 +16945,13 @@
         <v>1810</v>
       </c>
       <c r="H453" s="42" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="I453" s="4" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="K453" s="28" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="454" spans="1:11" ht="13">
@@ -16901,7 +16962,7 @@
         <v>98</v>
       </c>
       <c r="C454" s="29" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D454" s="23" t="s">
         <v>20</v>
@@ -16917,10 +16978,10 @@
         <v>1052</v>
       </c>
       <c r="I454" s="28" t="s">
+        <v>850</v>
+      </c>
+      <c r="K454" s="28" t="s">
         <v>851</v>
-      </c>
-      <c r="K454" s="28" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="455" spans="1:11" ht="13">
@@ -16942,13 +17003,13 @@
         <v>1810</v>
       </c>
       <c r="I455" s="28" t="s">
+        <v>852</v>
+      </c>
+      <c r="J455" s="28" t="s">
         <v>853</v>
       </c>
-      <c r="J455" s="28" t="s">
+      <c r="K455" s="28" t="s">
         <v>854</v>
-      </c>
-      <c r="K455" s="28" t="s">
-        <v>855</v>
       </c>
     </row>
     <row r="456" spans="1:11" ht="13">
@@ -16970,10 +17031,10 @@
         <v>1810</v>
       </c>
       <c r="I456" s="28" t="s">
+        <v>855</v>
+      </c>
+      <c r="K456" s="28" t="s">
         <v>856</v>
-      </c>
-      <c r="K456" s="28" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="457" spans="1:11" ht="13">
@@ -16987,7 +17048,7 @@
         <v>36</v>
       </c>
       <c r="D457" s="23" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="E457" s="26"/>
       <c r="F457" s="28" t="s">
@@ -16997,7 +17058,7 @@
         <v>1810</v>
       </c>
       <c r="K457" s="28" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="458" spans="1:11" ht="13">
@@ -17011,7 +17072,7 @@
         <v>71</v>
       </c>
       <c r="D458" s="23" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="E458" s="26"/>
       <c r="F458" s="28" t="s">
@@ -17021,10 +17082,10 @@
         <v>1810</v>
       </c>
       <c r="H458" s="42" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="K458" s="28" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="459" spans="1:11" ht="13">
@@ -17048,13 +17109,13 @@
         <v>1810</v>
       </c>
       <c r="H459" s="42" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="I459" s="28" t="s">
+        <v>861</v>
+      </c>
+      <c r="K459" s="28" t="s">
         <v>862</v>
-      </c>
-      <c r="K459" s="28" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="460" spans="1:11" ht="13">
@@ -17078,10 +17139,10 @@
         <v>1810</v>
       </c>
       <c r="I460" s="6" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="K460" s="28" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="461" spans="1:11" ht="13">
@@ -17092,7 +17153,7 @@
         <v>105</v>
       </c>
       <c r="C461" s="29" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D461" s="23" t="s">
         <v>20</v>
@@ -17105,10 +17166,10 @@
         <v>1810</v>
       </c>
       <c r="I461" s="28" t="s">
+        <v>865</v>
+      </c>
+      <c r="K461" s="28" t="s">
         <v>866</v>
-      </c>
-      <c r="K461" s="28" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="462" spans="1:11" ht="13">
@@ -17122,7 +17183,7 @@
         <v>23</v>
       </c>
       <c r="D462" s="23" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="E462" s="26"/>
       <c r="F462" s="28" t="s">
@@ -17132,7 +17193,7 @@
         <v>1810</v>
       </c>
       <c r="K462" s="28" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="463" spans="1:11" ht="13">
@@ -17143,10 +17204,10 @@
         <v>107</v>
       </c>
       <c r="C463" s="29" t="s">
+        <v>868</v>
+      </c>
+      <c r="D463" s="23" t="s">
         <v>869</v>
-      </c>
-      <c r="D463" s="23" t="s">
-        <v>870</v>
       </c>
       <c r="E463" s="26"/>
       <c r="F463" s="28" t="s">
@@ -17159,7 +17220,7 @@
         <v>1771</v>
       </c>
       <c r="K463" s="28" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="464" spans="1:11" ht="13">
@@ -17181,10 +17242,10 @@
         <v>1810</v>
       </c>
       <c r="I464" s="28" t="s">
+        <v>870</v>
+      </c>
+      <c r="K464" s="28" t="s">
         <v>871</v>
-      </c>
-      <c r="K464" s="28" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="465" spans="1:11" ht="13">
@@ -17208,10 +17269,10 @@
         <v>1810</v>
       </c>
       <c r="I465" s="28" t="s">
+        <v>872</v>
+      </c>
+      <c r="K465" s="28" t="s">
         <v>873</v>
-      </c>
-      <c r="K465" s="28" t="s">
-        <v>874</v>
       </c>
     </row>
     <row r="466" spans="1:11" ht="13">
@@ -17235,16 +17296,16 @@
         <v>1770</v>
       </c>
       <c r="H466" s="42" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="I466" s="28" t="s">
+        <v>874</v>
+      </c>
+      <c r="J466" s="28" t="s">
         <v>875</v>
       </c>
-      <c r="J466" s="28" t="s">
+      <c r="K466" s="28" t="s">
         <v>876</v>
-      </c>
-      <c r="K466" s="28" t="s">
-        <v>877</v>
       </c>
     </row>
     <row r="467" spans="1:11" ht="13">
@@ -17268,16 +17329,16 @@
         <v>1760</v>
       </c>
       <c r="H467" s="42" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="I467" s="28" t="s">
+        <v>874</v>
+      </c>
+      <c r="J467" s="28" t="s">
         <v>875</v>
       </c>
-      <c r="J467" s="28" t="s">
-        <v>876</v>
-      </c>
       <c r="K467" s="28" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="468" spans="1:11" ht="13">
@@ -17301,16 +17362,16 @@
         <v>1750</v>
       </c>
       <c r="H468" s="42" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="I468" s="28" t="s">
+        <v>874</v>
+      </c>
+      <c r="J468" s="28" t="s">
         <v>875</v>
       </c>
-      <c r="J468" s="28" t="s">
-        <v>876</v>
-      </c>
       <c r="K468" s="28" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="469" spans="1:11" ht="13">
@@ -17332,7 +17393,7 @@
         <v>1810</v>
       </c>
       <c r="K469" s="28" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="470" spans="1:11" ht="13">
@@ -17354,13 +17415,13 @@
         <v>1810</v>
       </c>
       <c r="H470" s="42" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="I470" s="28" t="s">
         <v>283</v>
       </c>
       <c r="K470" s="37" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="471" spans="1:11" ht="14">
@@ -17372,7 +17433,7 @@
       </c>
       <c r="C471" s="25"/>
       <c r="D471" s="23" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="E471" s="26"/>
       <c r="F471" s="28" t="s">
@@ -17382,13 +17443,13 @@
         <v>1810</v>
       </c>
       <c r="H471" s="42" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="J471" s="40" t="s">
+        <v>882</v>
+      </c>
+      <c r="K471" s="28" t="s">
         <v>883</v>
-      </c>
-      <c r="K471" s="28" t="s">
-        <v>884</v>
       </c>
     </row>
     <row r="472" spans="1:11" ht="13">
@@ -17412,7 +17473,7 @@
         <v>1810</v>
       </c>
       <c r="H472" s="42" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="I472" s="28" t="s">
         <v>716</v>
@@ -17448,7 +17509,7 @@
         <v>719</v>
       </c>
       <c r="K473" s="28" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="474" spans="1:11" ht="13">
@@ -17470,7 +17531,7 @@
         <v>1810</v>
       </c>
       <c r="K474" s="28" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="475" spans="1:11" ht="13">
@@ -17492,10 +17553,10 @@
         <v>1810</v>
       </c>
       <c r="I475" s="4" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="K475" s="28" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="476" spans="1:11" ht="13">
@@ -17517,10 +17578,10 @@
         <v>1810</v>
       </c>
       <c r="I476" s="28" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="K476" s="37" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="477" spans="1:11" ht="13">
@@ -17534,7 +17595,7 @@
         <v>319</v>
       </c>
       <c r="D477" s="23" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E477" s="26"/>
       <c r="F477" s="28" t="s">
@@ -17550,7 +17611,7 @@
         <v>730</v>
       </c>
       <c r="K477" s="28" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="478" spans="1:11" ht="13">
@@ -17564,7 +17625,7 @@
         <v>36</v>
       </c>
       <c r="D478" s="23" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E478" s="26"/>
       <c r="F478" s="28" t="s">
@@ -17574,10 +17635,10 @@
         <v>1810</v>
       </c>
       <c r="H478" s="42" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="K478" s="28" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="479" spans="1:11" ht="13">
@@ -17599,10 +17660,10 @@
         <v>1810</v>
       </c>
       <c r="I479" s="28" t="s">
+        <v>891</v>
+      </c>
+      <c r="K479" s="37" t="s">
         <v>892</v>
-      </c>
-      <c r="K479" s="37" t="s">
-        <v>893</v>
       </c>
     </row>
     <row r="480" spans="1:11" ht="13">
@@ -17638,7 +17699,7 @@
       </c>
       <c r="C481" s="25"/>
       <c r="D481" s="23" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E481" s="26"/>
       <c r="F481" s="28" t="s">
@@ -17648,7 +17709,7 @@
         <v>1800</v>
       </c>
       <c r="K481" s="28" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="482" spans="1:11" ht="13">
@@ -17672,13 +17733,13 @@
         <v>1810</v>
       </c>
       <c r="H482" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="J482" s="28" t="s">
+        <v>895</v>
+      </c>
+      <c r="K482" s="28" t="s">
         <v>896</v>
-      </c>
-      <c r="K482" s="28" t="s">
-        <v>897</v>
       </c>
     </row>
     <row r="483" spans="1:11" ht="13">
@@ -17702,10 +17763,10 @@
         <v>1810</v>
       </c>
       <c r="I483" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="K483" s="28" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="484" spans="1:11" ht="13">
@@ -17729,13 +17790,13 @@
         <v>1810</v>
       </c>
       <c r="I484" s="28" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="J484" s="28" t="s">
         <v>397</v>
       </c>
       <c r="K484" s="28" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="485" spans="1:11" ht="13">
@@ -17746,7 +17807,7 @@
         <v>129</v>
       </c>
       <c r="C485" s="29" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="D485" s="23" t="s">
         <v>20</v>
@@ -17762,13 +17823,13 @@
         <v>5004</v>
       </c>
       <c r="I485" s="28" t="s">
+        <v>901</v>
+      </c>
+      <c r="J485" s="36" t="s">
         <v>902</v>
       </c>
-      <c r="J485" s="36" t="s">
+      <c r="K485" s="37" t="s">
         <v>903</v>
-      </c>
-      <c r="K485" s="37" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="486" spans="1:11" ht="13">
@@ -17790,10 +17851,10 @@
         <v>1810</v>
       </c>
       <c r="I486" s="28" t="s">
+        <v>904</v>
+      </c>
+      <c r="K486" s="37" t="s">
         <v>905</v>
-      </c>
-      <c r="K486" s="37" t="s">
-        <v>906</v>
       </c>
     </row>
     <row r="487" spans="1:11" ht="13">
@@ -17807,7 +17868,7 @@
         <v>50</v>
       </c>
       <c r="D487" s="23" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E487" s="26"/>
       <c r="F487" s="28" t="s">
@@ -17817,10 +17878,10 @@
         <v>1810</v>
       </c>
       <c r="J487" s="28" t="s">
+        <v>907</v>
+      </c>
+      <c r="K487" s="28" t="s">
         <v>908</v>
-      </c>
-      <c r="K487" s="28" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="488" spans="1:11" ht="13">
@@ -17842,7 +17903,7 @@
         <v>1810</v>
       </c>
       <c r="K488" s="28" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="489" spans="1:11" ht="13">
@@ -17853,7 +17914,7 @@
         <v>133</v>
       </c>
       <c r="C489" s="29" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="D489" s="23" t="s">
         <v>584</v>
@@ -17866,10 +17927,10 @@
         <v>1810</v>
       </c>
       <c r="J489" s="28" t="s">
+        <v>911</v>
+      </c>
+      <c r="K489" s="28" t="s">
         <v>912</v>
-      </c>
-      <c r="K489" s="28" t="s">
-        <v>913</v>
       </c>
     </row>
     <row r="490" spans="1:11" ht="13">
@@ -17880,10 +17941,10 @@
         <v>134</v>
       </c>
       <c r="C490" s="29" t="s">
+        <v>913</v>
+      </c>
+      <c r="D490" s="23" t="s">
         <v>914</v>
-      </c>
-      <c r="D490" s="23" t="s">
-        <v>915</v>
       </c>
       <c r="E490" s="26"/>
       <c r="F490" s="39" t="s">
@@ -17893,7 +17954,7 @@
         <v>1810</v>
       </c>
       <c r="K490" s="37" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="491" spans="1:11" ht="13">
@@ -17907,7 +17968,7 @@
         <v>609</v>
       </c>
       <c r="D491" s="23" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E491" s="26"/>
       <c r="F491" s="37" t="s">
@@ -17916,11 +17977,14 @@
       <c r="G491" s="30">
         <v>1810</v>
       </c>
+      <c r="H491" s="42" t="s">
+        <v>979</v>
+      </c>
       <c r="J491" s="37" t="s">
+        <v>917</v>
+      </c>
+      <c r="K491" s="37" t="s">
         <v>918</v>
-      </c>
-      <c r="K491" s="37" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="492" spans="1:11" ht="13">
@@ -17944,13 +18008,13 @@
         <v>1810</v>
       </c>
       <c r="H492" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I492" s="28" t="s">
+        <v>919</v>
+      </c>
+      <c r="K492" s="37" t="s">
         <v>920</v>
-      </c>
-      <c r="K492" s="37" t="s">
-        <v>921</v>
       </c>
     </row>
     <row r="493" spans="1:11" ht="13">
@@ -17981,7 +18045,7 @@
         <v>616</v>
       </c>
       <c r="K493" s="37" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="494" spans="1:11" ht="13">
@@ -18022,7 +18086,7 @@
         <v>141</v>
       </c>
       <c r="C495" s="29" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D495" s="23" t="s">
         <v>20</v>
@@ -18035,10 +18099,10 @@
         <v>1810</v>
       </c>
       <c r="I495" s="28" t="s">
+        <v>923</v>
+      </c>
+      <c r="K495" s="37" t="s">
         <v>924</v>
-      </c>
-      <c r="K495" s="37" t="s">
-        <v>925</v>
       </c>
     </row>
     <row r="496" spans="1:11" ht="13">
@@ -18063,13 +18127,13 @@
         <v>5385</v>
       </c>
       <c r="I496" s="28" t="s">
+        <v>925</v>
+      </c>
+      <c r="J496" s="28" t="s">
         <v>926</v>
       </c>
-      <c r="J496" s="28" t="s">
+      <c r="K496" s="37" t="s">
         <v>927</v>
-      </c>
-      <c r="K496" s="37" t="s">
-        <v>928</v>
       </c>
     </row>
     <row r="497" spans="1:11" ht="13">
@@ -18092,17 +18156,15 @@
       <c r="G497" s="30">
         <v>1810</v>
       </c>
-      <c r="H497" s="42" t="s">
-        <v>993</v>
-      </c>
+      <c r="H497" s="42"/>
       <c r="I497" s="28" t="s">
+        <v>928</v>
+      </c>
+      <c r="J497" s="36" t="s">
         <v>929</v>
       </c>
-      <c r="J497" s="36" t="s">
+      <c r="K497" s="28" t="s">
         <v>930</v>
-      </c>
-      <c r="K497" s="28" t="s">
-        <v>931</v>
       </c>
     </row>
     <row r="498" spans="1:11" ht="13">
@@ -18114,14 +18176,14 @@
       </c>
       <c r="C498" s="25"/>
       <c r="D498" s="23" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="E498" s="26"/>
       <c r="G498" s="30">
         <v>1810</v>
       </c>
       <c r="K498" s="37" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="499" spans="1:11" ht="13">
@@ -18146,13 +18208,13 @@
         <v>5504</v>
       </c>
       <c r="I499" s="28" t="s">
+        <v>933</v>
+      </c>
+      <c r="J499" s="36" t="s">
         <v>934</v>
       </c>
-      <c r="J499" s="36" t="s">
+      <c r="K499" s="37" t="s">
         <v>935</v>
-      </c>
-      <c r="K499" s="37" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="500" spans="1:11" ht="13">
@@ -18164,14 +18226,14 @@
       </c>
       <c r="C500" s="25"/>
       <c r="D500" s="23" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="E500" s="26"/>
       <c r="G500" s="30">
         <v>1810</v>
       </c>
       <c r="K500" s="37" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="501" spans="1:11" ht="13">
@@ -18196,13 +18258,13 @@
         <v>5505</v>
       </c>
       <c r="I501" s="28" t="s">
+        <v>938</v>
+      </c>
+      <c r="J501" s="36" t="s">
         <v>939</v>
       </c>
-      <c r="J501" s="36" t="s">
+      <c r="K501" s="37" t="s">
         <v>940</v>
-      </c>
-      <c r="K501" s="37" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="502" spans="1:11" ht="13">
@@ -18226,10 +18288,10 @@
         <v>1810</v>
       </c>
       <c r="I502" s="6" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="K502" s="37" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="503" spans="1:11" ht="13">
@@ -18240,17 +18302,17 @@
         <v>149</v>
       </c>
       <c r="C503" s="29" t="s">
+        <v>942</v>
+      </c>
+      <c r="D503" s="23" t="s">
         <v>943</v>
-      </c>
-      <c r="D503" s="23" t="s">
-        <v>944</v>
       </c>
       <c r="E503" s="26"/>
       <c r="G503" s="30">
         <v>1810</v>
       </c>
       <c r="K503" s="37" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="504" spans="1:11" ht="13">
@@ -18264,14 +18326,14 @@
         <v>36</v>
       </c>
       <c r="D504" s="23" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="E504" s="26"/>
       <c r="G504" s="30">
         <v>1810</v>
       </c>
       <c r="K504" s="37" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="505" spans="1:11" ht="13">
@@ -18283,14 +18345,14 @@
       </c>
       <c r="C505" s="25"/>
       <c r="D505" s="23" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="E505" s="26"/>
       <c r="G505" s="30">
         <v>1810</v>
       </c>
       <c r="K505" s="37" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="506" spans="1:11" ht="13">
@@ -18301,17 +18363,17 @@
         <v>152</v>
       </c>
       <c r="C506" s="29" t="s">
+        <v>948</v>
+      </c>
+      <c r="D506" s="23" t="s">
         <v>949</v>
-      </c>
-      <c r="D506" s="23" t="s">
-        <v>950</v>
       </c>
       <c r="E506" s="26"/>
       <c r="G506" s="30">
         <v>1810</v>
       </c>
       <c r="K506" s="37" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="507" spans="1:11" ht="13">
@@ -18322,15 +18384,21 @@
         <v>153</v>
       </c>
       <c r="C507" s="25"/>
-      <c r="D507" s="23" t="s">
-        <v>779</v>
+      <c r="D507" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="E507" s="26"/>
+      <c r="F507" t="s">
+        <v>296</v>
+      </c>
       <c r="G507" s="30">
         <v>1810</v>
       </c>
+      <c r="I507" t="s">
+        <v>1057</v>
+      </c>
       <c r="K507" s="37" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="508" spans="1:11" ht="13">
@@ -18342,14 +18410,14 @@
       </c>
       <c r="C508" s="25"/>
       <c r="D508" s="23" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="E508" s="26"/>
       <c r="G508" s="30">
         <v>1810</v>
       </c>
       <c r="K508" s="37" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="509" spans="1:11" ht="13">
@@ -18363,14 +18431,14 @@
         <v>619</v>
       </c>
       <c r="D509" s="23" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="E509" s="26"/>
       <c r="G509" s="30">
         <v>1810</v>
       </c>
       <c r="K509" s="28" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="510" spans="1:11" ht="13">
@@ -18392,16 +18460,16 @@
         <v>1810</v>
       </c>
       <c r="H510" s="28" t="s">
+        <v>956</v>
+      </c>
+      <c r="I510" s="28" t="s">
         <v>957</v>
       </c>
-      <c r="I510" s="28" t="s">
+      <c r="J510" s="28" t="s">
         <v>958</v>
       </c>
-      <c r="J510" s="28" t="s">
+      <c r="K510" s="37" t="s">
         <v>959</v>
-      </c>
-      <c r="K510" s="37" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="511" spans="1:11" ht="13">
@@ -18413,7 +18481,7 @@
       </c>
       <c r="C511" s="25"/>
       <c r="D511" s="23" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E511" s="26"/>
       <c r="G511" s="30">
@@ -18423,7 +18491,7 @@
         <v>5818</v>
       </c>
       <c r="K511" s="37" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="512" spans="1:11" ht="13">
@@ -18448,10 +18516,10 @@
         <v>5828</v>
       </c>
       <c r="I512" s="28" t="s">
+        <v>962</v>
+      </c>
+      <c r="K512" s="37" t="s">
         <v>963</v>
-      </c>
-      <c r="K512" s="37" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="513" spans="1:11" ht="13">
@@ -18463,14 +18531,14 @@
       </c>
       <c r="C513" s="25"/>
       <c r="D513" s="23" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="E513" s="26"/>
       <c r="G513" s="30">
         <v>1810</v>
       </c>
       <c r="K513" s="37" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="514" spans="1:11" ht="13">
@@ -18497,13 +18565,13 @@
         <v>678</v>
       </c>
       <c r="I514" s="28" t="s">
+        <v>966</v>
+      </c>
+      <c r="J514" s="28" t="s">
         <v>967</v>
       </c>
-      <c r="J514" s="28" t="s">
+      <c r="K514" s="37" t="s">
         <v>968</v>
-      </c>
-      <c r="K514" s="37" t="s">
-        <v>969</v>
       </c>
     </row>
     <row r="515" spans="1:11" ht="13">

</xml_diff>

<commit_message>
Updates, fixes and new stations
</commit_message>
<xml_diff>
--- a/LOCATION SHEETS/1677sLOCATIONS.xlsx
+++ b/LOCATION SHEETS/1677sLOCATIONS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Documents/WR4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4DC48E-6214-7345-A248-AF17248633C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4086273A-873B-C54E-B421-928236C1C123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="460" windowWidth="28100" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2740" yWindow="500" windowWidth="28100" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1677sLOCATIONS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="1058">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="1057">
   <si>
     <t>LOCATIONS FOR MIXTURE OF DECADES</t>
   </si>
@@ -4088,9 +4088,6 @@
   </si>
   <si>
     <t>Chelmsford (BRITTON)</t>
-  </si>
-  <si>
-    <t>EDINBURGH UNKNOWN</t>
   </si>
   <si>
     <t>RR502</t>
@@ -4896,8 +4893,8 @@
   <dimension ref="A1:K1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A471" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I491" sqref="I491"/>
+      <pane ySplit="6" topLeftCell="A484" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F506" sqref="F506"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -6700,7 +6697,7 @@
         <v>1780</v>
       </c>
       <c r="H68" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="K68" s="28" t="s">
         <v>142</v>
@@ -6725,7 +6722,7 @@
         <v>1790</v>
       </c>
       <c r="H69" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="K69" s="28" t="s">
         <v>143</v>
@@ -6772,7 +6769,7 @@
         <v>1780</v>
       </c>
       <c r="H71" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="K71" s="28" t="s">
         <v>147</v>
@@ -7578,7 +7575,7 @@
         <v>1740</v>
       </c>
       <c r="H100" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="K100" s="28" t="s">
         <v>213</v>
@@ -7604,7 +7601,7 @@
       </c>
       <c r="H101" s="42"/>
       <c r="I101" s="42" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="K101" s="28" t="s">
         <v>214</v>
@@ -7689,7 +7686,7 @@
         <v>1790</v>
       </c>
       <c r="H104" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="K104" s="28" t="s">
         <v>222</v>
@@ -7714,7 +7711,7 @@
         <v>1790</v>
       </c>
       <c r="H105" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="K105" s="28" t="s">
         <v>223</v>
@@ -13162,7 +13159,7 @@
         <v>1770</v>
       </c>
       <c r="H306" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="I306" s="28" t="s">
         <v>579</v>
@@ -13193,7 +13190,7 @@
         <v>1770</v>
       </c>
       <c r="H307" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="I307" s="28" t="s">
         <v>582</v>
@@ -13268,7 +13265,7 @@
         <v>1780</v>
       </c>
       <c r="H310" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="I310" s="28" t="s">
         <v>587</v>
@@ -13298,7 +13295,7 @@
         <v>1790</v>
       </c>
       <c r="H311" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="I311" s="6" t="s">
         <v>587</v>
@@ -13435,7 +13432,7 @@
         <v>1800</v>
       </c>
       <c r="I316" t="s">
-        <v>1050</v>
+        <v>584</v>
       </c>
       <c r="K316" s="28" t="s">
         <v>599</v>
@@ -14140,7 +14137,7 @@
       <c r="C343" s="29" t="s">
         <v>653</v>
       </c>
-      <c r="D343" s="23" t="s">
+      <c r="D343" s="4" t="s">
         <v>654</v>
       </c>
       <c r="E343" s="26"/>
@@ -15962,7 +15959,7 @@
         <v>1800</v>
       </c>
       <c r="I414" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="K414" s="28" t="s">
         <v>779</v>
@@ -18344,7 +18341,7 @@
         <v>151</v>
       </c>
       <c r="C505" s="25"/>
-      <c r="D505" s="23" t="s">
+      <c r="D505" s="4" t="s">
         <v>946</v>
       </c>
       <c r="E505" s="26"/>
@@ -18395,7 +18392,7 @@
         <v>1810</v>
       </c>
       <c r="I507" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="K507" s="37" t="s">
         <v>951</v>

</xml_diff>